<commit_message>
heat pad added to frame calculator
</commit_message>
<xml_diff>
--- a/FrameCalculator.xlsx
+++ b/FrameCalculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="114_{04D01490-EE98-4F05-8C12-A1B4D3BC434B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5A9FBC0B-2B4D-4C71-9F97-3A6BB1C3A4A4}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="114_{04D01490-EE98-4F05-8C12-A1B4D3BC434B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{36AD52A6-797C-48EA-AEF9-AD62A59D2BA6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{2DD4E541-7648-4A97-AB5A-A9C0E0660C31}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2DD4E541-7648-4A97-AB5A-A9C0E0660C31}"/>
   </bookViews>
   <sheets>
     <sheet name="FRAMECALCULATOR" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="18" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="129">
   <si>
     <t>Desired Print Area</t>
   </si>
@@ -216,9 +216,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>MIC6 Alu 6mm</t>
-  </si>
-  <si>
     <t>XHHF</t>
   </si>
   <si>
@@ -402,9 +399,6 @@
     <t>GT2 Belt</t>
   </si>
   <si>
-    <t>As eneterd on the previous sheet:</t>
-  </si>
-  <si>
     <t>Bed Size</t>
   </si>
   <si>
@@ -412,6 +406,27 @@
   </si>
   <si>
     <t>mm</t>
+  </si>
+  <si>
+    <t>ZR_HeaterPad</t>
+  </si>
+  <si>
+    <t>ZR_SiliconeHeatPad</t>
+  </si>
+  <si>
+    <t>Silicone Heat Pad (Keenovo Recommended)</t>
+  </si>
+  <si>
+    <t>SiliconeHeatPad (Square)</t>
+  </si>
+  <si>
+    <t>MIC6 Alu 6mm (Square)</t>
+  </si>
+  <si>
+    <t>Heated Pad recommended size</t>
+  </si>
+  <si>
+    <t>As entered on the previous sheet:</t>
   </si>
 </sst>
 </file>
@@ -568,12 +583,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -593,6 +602,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1044,11 +1059,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1056,22 +1070,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1098,221 +1112,142 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general"/>
+  <dxfs count="150">
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
     </dxf>
     <dxf>
       <fill>
@@ -1343,22 +1278,218 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom"/>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
     </dxf>
     <dxf>
       <border>
@@ -1471,16 +1602,1380 @@
       </border>
     </dxf>
     <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF33CCFF"/>
       <color rgb="FFEBFC96"/>
       <color rgb="FFD1F810"/>
       <color rgb="FF00FFFF"/>
-      <color rgb="FF33CCFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1548,23 +3043,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>527050</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>612322</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>27215</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>16165</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>69398</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>73565</xdr:rowOff>
+      <xdr:rowOff>182336</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B842143-C9D1-4021-AD05-10C5B18931FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{320ABF8F-B871-47FF-ABBB-1FE2D4C2E4E0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1587,8 +3082,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="14255750" y="1273175"/>
-          <a:ext cx="8010814" cy="8039296"/>
+          <a:off x="14967858" y="1306286"/>
+          <a:ext cx="7621361" cy="8768443"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1622,8 +3117,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>515541</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1666,9 +3161,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Olivier Royer-Tardif" refreshedDate="44048.690906481483" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="43" xr:uid="{EE21856B-4584-42FE-9CE7-DE41726CCFEE}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Olivier Royer-Tardif" refreshedDate="44082.589951388887" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="44" xr:uid="{9DE3B3A4-4E52-4408-AE9E-80A17BDCAD77}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="C7:H50" sheet="FRAMECALCULATOR"/>
+    <worksheetSource ref="C7:H51" sheet="FRAMECALCULATOR"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Structure Section" numFmtId="0">
@@ -1681,18 +3176,21 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Part Type" numFmtId="0">
-      <sharedItems count="7">
+      <sharedItems count="10">
         <s v="3030 Extrusion"/>
         <s v="2020 Extrusion"/>
-        <s v="MIC6 Alu 6mm"/>
+        <s v="MIC6 Alu 6mm (Square)"/>
         <s v="MGN12C Rail"/>
         <s v="MGN12H Rail"/>
         <s v="SFU1204 Screw"/>
         <s v="GT2 Belt"/>
+        <s v="SiliconeHeatPad (Square)"/>
+        <s v="SiliconeHeatPad" u="1"/>
+        <s v="MIC6 Alu 6mm" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Length mm" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="140" maxValue="6400" count="56">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="140" maxValue="4000" count="15">
         <n v="420"/>
         <n v="410"/>
         <n v="880"/>
@@ -1707,48 +3205,7 @@
         <n v="450"/>
         <n v="150"/>
         <n v="4000"/>
-        <n v="440" u="1"/>
-        <n v="710" u="1"/>
-        <n v="1080" u="1"/>
-        <n v="485" u="1"/>
-        <n v="600" u="1"/>
-        <n v="1170" u="1"/>
-        <n v="716" u="1"/>
-        <n v="4800" u="1"/>
-        <n v="6400" u="1"/>
-        <n v="1130" u="1"/>
-        <n v="625" u="1"/>
-        <n v="980" u="1"/>
-        <n v="670" u="1"/>
-        <n v="560" u="1"/>
-        <n v="631" u="1"/>
-        <n v="760" u="1"/>
-        <n v="605" u="1"/>
-        <n v="650" u="1"/>
-        <n v="695" u="1"/>
-        <n v="540" u="1"/>
-        <n v="585" u="1"/>
-        <n v="1140" u="1"/>
-        <n v="1540" u="1"/>
-        <n v="500" u="1"/>
-        <n v="6280" u="1"/>
-        <n v="520" u="1"/>
-        <n v="720" u="1"/>
-        <n v="610" u="1"/>
-        <n v="700" u="1"/>
-        <n v="545" u="1"/>
-        <n v="5600" u="1"/>
-        <n v="1110" u="1"/>
-        <n v="770" u="1"/>
-        <n v="531" u="1"/>
-        <n v="731" u="1"/>
-        <n v="360" u="1"/>
-        <n v="705" u="1"/>
-        <n v="460" u="1"/>
-        <n v="550" u="1"/>
-        <n v="640" u="1"/>
-        <n v="685" u="1"/>
-        <n v="620" u="1"/>
+        <n v="300"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Qty" numFmtId="0">
@@ -1764,7 +3221,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="43">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="44">
   <r>
     <s v="Frame"/>
     <s v="HHB"/>
@@ -2109,25 +3566,36 @@
     <x v="13"/>
     <n v="1"/>
   </r>
+  <r>
+    <s v="ZR_HeaterPad"/>
+    <s v="ZR_SiliconeHeatPad"/>
+    <s v="Silicone Heat Pad (Keenovo Recommended)"/>
+    <x v="7"/>
+    <x v="14"/>
+    <n v="1"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{94C6CC85-CA6D-48DC-B3E5-974B9FFE69AC}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" showDataTips="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="O7:Q30" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BDCFAFF3-D92B-420B-A37D-3E3E68134BAA}" name="PivotTable2" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" showDataTips="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="O7:Q32" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" insertBlankRow="1" defaultSubtotal="0">
-      <items count="7">
+      <items count="10">
         <item x="1"/>
         <item x="0"/>
         <item x="3"/>
         <item x="4"/>
-        <item x="2"/>
+        <item m="1" x="9"/>
         <item x="5"/>
         <item x="6"/>
+        <item m="1" x="8"/>
+        <item x="2"/>
+        <item x="7"/>
       </items>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
@@ -2136,7 +3604,7 @@
       </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="57">
+      <items count="16">
         <item x="12"/>
         <item x="5"/>
         <item x="6"/>
@@ -2151,48 +3619,7 @@
         <item x="2"/>
         <item x="4"/>
         <item x="13"/>
-        <item m="1" x="55"/>
-        <item m="1" x="41"/>
-        <item m="1" x="51"/>
-        <item m="1" x="39"/>
-        <item m="1" x="28"/>
-        <item m="1" x="33"/>
-        <item m="1" x="18"/>
-        <item m="1" x="34"/>
-        <item m="1" x="44"/>
-        <item m="1" x="16"/>
-        <item m="1" x="15"/>
-        <item m="1" x="31"/>
-        <item m="1" x="23"/>
-        <item m="1" x="29"/>
-        <item m="1" x="42"/>
-        <item m="1" x="25"/>
-        <item m="1" x="49"/>
-        <item m="1" x="47"/>
-        <item m="1" x="14"/>
-        <item m="1" x="37"/>
-        <item m="1" x="17"/>
-        <item m="1" x="52"/>
-        <item m="1" x="21"/>
-        <item m="1" x="40"/>
-        <item m="1" x="27"/>
-        <item m="1" x="48"/>
-        <item m="1" x="53"/>
-        <item m="1" x="54"/>
-        <item m="1" x="22"/>
-        <item m="1" x="50"/>
-        <item m="1" x="32"/>
-        <item m="1" x="35"/>
-        <item m="1" x="46"/>
-        <item m="1" x="43"/>
-        <item m="1" x="30"/>
-        <item m="1" x="20"/>
-        <item m="1" x="24"/>
-        <item m="1" x="26"/>
-        <item m="1" x="38"/>
-        <item m="1" x="36"/>
-        <item m="1" x="19"/>
-        <item m="1" x="45"/>
+        <item x="14"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2202,7 +3629,7 @@
     <field x="3"/>
     <field x="4"/>
   </rowFields>
-  <rowItems count="22">
+  <rowItems count="24">
     <i>
       <x/>
       <x v="1"/>
@@ -2256,13 +3683,6 @@
       <x v="3"/>
     </i>
     <i>
-      <x v="4"/>
-      <x v="3"/>
-    </i>
-    <i t="blank">
-      <x v="4"/>
-    </i>
-    <i>
       <x v="5"/>
       <x v="8"/>
     </i>
@@ -2276,6 +3696,20 @@
     <i t="blank">
       <x v="6"/>
     </i>
+    <i>
+      <x v="8"/>
+      <x v="3"/>
+    </i>
+    <i t="blank">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x v="14"/>
+    </i>
+    <i t="blank">
+      <x v="9"/>
+    </i>
   </rowItems>
   <colItems count="1">
     <i/>
@@ -2284,80 +3718,80 @@
     <dataField name="Sum of Qty" fld="5" baseField="4" baseItem="2"/>
   </dataFields>
   <formats count="30">
-    <format dxfId="29">
+    <format dxfId="90">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="91">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="92">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="93">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="94">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="95">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="96">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="97">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="98">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="99">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="100">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="101">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="102">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="103">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="104">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="105">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="13">
+    <format dxfId="106">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="107">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="108">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="109">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="110">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="111">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="112">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="113">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -2370,7 +3804,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="114">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -2384,7 +3818,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="115">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -2396,7 +3830,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="116">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -2410,7 +3844,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="117">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -2422,7 +3856,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="118">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -2434,7 +3868,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="119">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -2750,10 +4184,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="B1:U50"/>
+  <dimension ref="B1:U51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2763,17 +4197,18 @@
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="8.140625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="4.140625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="12.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="8.140625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="9.140625" collapsed="1"/>
     <col min="13" max="13" width="11.85546875" customWidth="1"/>
     <col min="14" max="14" width="1.28515625" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.140625" customWidth="1"/>
     <col min="19" max="19" width="12.28515625" customWidth="1"/>
   </cols>
@@ -2796,7 +4231,7 @@
         <v>315</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="3:21" ht="18.75" x14ac:dyDescent="0.3">
@@ -2821,23 +4256,23 @@
         <v>340</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="3:21" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="U5" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="3:21" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="O6" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="O6" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="59"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="58"/>
     </row>
     <row r="7" spans="3:21" s="12" customFormat="1" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="8" t="s">
@@ -2888,7 +4323,7 @@
         <v>19</v>
       </c>
       <c r="G8" s="14">
-        <f t="shared" ref="G8:G49" si="0">IFERROR(VLOOKUP(I8,$E$2:$F$4,2,0),0)+K8</f>
+        <f t="shared" ref="G8:G51" si="0">IFERROR(VLOOKUP(I8,$E$2:$F$4,2,0),0)+K8</f>
         <v>420</v>
       </c>
       <c r="H8" s="14">
@@ -3542,10 +4977,10 @@
         <v>52</v>
       </c>
       <c r="D25" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>60</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>19</v>
@@ -3568,13 +5003,13 @@
       </c>
       <c r="N25" s="24"/>
       <c r="O25" s="40" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="P25" s="40">
-        <v>340</v>
+        <v>450</v>
       </c>
       <c r="Q25" s="31">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3583,10 +5018,10 @@
         <v>52</v>
       </c>
       <c r="D26" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>19</v>
@@ -3618,10 +5053,10 @@
         <v>52</v>
       </c>
       <c r="D27" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>64</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>65</v>
       </c>
       <c r="F27" s="14" t="s">
         <v>19</v>
@@ -3644,13 +5079,13 @@
       </c>
       <c r="N27" s="24"/>
       <c r="O27" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="P27" s="40">
-        <v>450</v>
+        <v>118</v>
+      </c>
+      <c r="P27" s="15">
+        <v>4000</v>
       </c>
       <c r="Q27" s="31">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3659,10 +5094,10 @@
         <v>52</v>
       </c>
       <c r="D28" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="13" t="s">
         <v>66</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>67</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>19</v>
@@ -3693,10 +5128,10 @@
         <v>52</v>
       </c>
       <c r="D29" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="13" t="s">
         <v>68</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>69</v>
       </c>
       <c r="F29" s="14" t="s">
         <v>19</v>
@@ -3718,12 +5153,12 @@
         <v>540</v>
       </c>
       <c r="L29" s="1"/>
-      <c r="N29" s="43"/>
+      <c r="N29" s="24"/>
       <c r="O29" s="40" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="P29" s="15">
-        <v>4000</v>
+        <v>340</v>
       </c>
       <c r="Q29" s="31">
         <v>1</v>
@@ -3735,10 +5170,10 @@
         <v>52</v>
       </c>
       <c r="D30" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="13" t="s">
         <v>70</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>71</v>
       </c>
       <c r="F30" s="14" t="s">
         <v>19</v>
@@ -3759,20 +5194,20 @@
       <c r="K30" s="1">
         <v>540</v>
       </c>
-      <c r="O30" s="27"/>
-      <c r="P30" s="28"/>
-      <c r="Q30" s="32"/>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O30" s="26"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="31"/>
+    </row>
+    <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="24"/>
       <c r="C31" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="E31" s="13" t="s">
         <v>73</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>74</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>19</v>
@@ -3793,19 +5228,27 @@
       <c r="K31" s="1">
         <v>170</v>
       </c>
-      <c r="P31"/>
-      <c r="Q31"/>
-    </row>
-    <row r="32" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="N31" s="62"/>
+      <c r="O31" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="P31" s="15">
+        <v>300</v>
+      </c>
+      <c r="Q31" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="24"/>
       <c r="C32" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D32" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="13" t="s">
         <v>75</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>76</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>19</v>
@@ -3826,22 +5269,20 @@
       <c r="K32" s="1">
         <v>170</v>
       </c>
-      <c r="N32" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="P32" s="1"/>
-      <c r="Q32"/>
-    </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="O32" s="27"/>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="32"/>
+    </row>
+    <row r="33" spans="2:20" ht="21" x14ac:dyDescent="0.35">
       <c r="B33" s="24"/>
       <c r="C33" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>78</v>
       </c>
       <c r="F33" s="14" t="s">
         <v>19</v>
@@ -3862,18 +5303,21 @@
       <c r="K33" s="1">
         <v>170</v>
       </c>
+      <c r="N33" s="18" t="s">
+        <v>110</v>
+      </c>
       <c r="P33" s="1"/>
       <c r="Q33"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C34" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="E34" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>81</v>
       </c>
       <c r="F34" s="14" t="s">
         <v>23</v>
@@ -3900,13 +5344,13 @@
     </row>
     <row r="35" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C35" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D35" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="13" t="s">
         <v>82</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>83</v>
       </c>
       <c r="F35" s="14" t="s">
         <v>23</v>
@@ -3928,7 +5372,7 @@
         <v>-55</v>
       </c>
       <c r="M35" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N35" s="20"/>
       <c r="O35" s="20"/>
@@ -3940,13 +5384,13 @@
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C36" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" s="13" t="s">
         <v>84</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="F36" s="14" t="s">
         <v>23</v>
@@ -3967,26 +5411,26 @@
       <c r="K36" s="1">
         <v>5</v>
       </c>
-      <c r="M36" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="N36" s="60"/>
-      <c r="O36" s="60"/>
-      <c r="P36" s="60"/>
-      <c r="Q36" s="60"/>
-      <c r="R36" s="60"/>
-      <c r="S36" s="60"/>
-      <c r="T36" s="60"/>
+      <c r="M36" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="N36" s="59"/>
+      <c r="O36" s="59"/>
+      <c r="P36" s="59"/>
+      <c r="Q36" s="59"/>
+      <c r="R36" s="59"/>
+      <c r="S36" s="59"/>
+      <c r="T36" s="59"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C37" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D37" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" s="13" t="s">
         <v>86</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>87</v>
       </c>
       <c r="F37" s="14" t="s">
         <v>23</v>
@@ -4007,25 +5451,25 @@
       <c r="K37" s="1">
         <v>5</v>
       </c>
-      <c r="M37" s="60"/>
-      <c r="N37" s="60"/>
-      <c r="O37" s="60"/>
-      <c r="P37" s="60"/>
-      <c r="Q37" s="60"/>
-      <c r="R37" s="60"/>
-      <c r="S37" s="60"/>
-      <c r="T37" s="60"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+      <c r="O37" s="59"/>
+      <c r="P37" s="59"/>
+      <c r="Q37" s="59"/>
+      <c r="R37" s="59"/>
+      <c r="S37" s="59"/>
+      <c r="T37" s="59"/>
     </row>
     <row r="38" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="24"/>
       <c r="C38" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="E38" s="13" t="s">
         <v>113</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>114</v>
       </c>
       <c r="F38" s="14" t="s">
         <v>23</v>
@@ -4057,16 +5501,16 @@
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C39" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>89</v>
-      </c>
       <c r="F39" s="14" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="G39" s="14">
         <f t="shared" si="0"/>
@@ -4084,10 +5528,10 @@
       <c r="K39" s="1">
         <v>25</v>
       </c>
-      <c r="M39" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="N39" s="62"/>
+      <c r="M39" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="N39" s="61"/>
       <c r="O39" s="19" t="s">
         <v>5</v>
       </c>
@@ -4095,13 +5539,13 @@
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" s="42"/>
       <c r="C40" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="E40" s="13" t="s">
         <v>91</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>92</v>
       </c>
       <c r="F40" s="14" t="s">
         <v>42</v>
@@ -4122,10 +5566,10 @@
       <c r="K40" s="1">
         <v>85</v>
       </c>
-      <c r="M40" s="55">
+      <c r="M40" s="54">
         <v>315</v>
       </c>
-      <c r="N40" s="56"/>
+      <c r="N40" s="55"/>
       <c r="O40" s="16">
         <v>340</v>
       </c>
@@ -4133,13 +5577,13 @@
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="42"/>
       <c r="C41" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F41" s="14" t="s">
         <v>42</v>
@@ -4160,11 +5604,11 @@
       <c r="K41" s="1">
         <v>85</v>
       </c>
-      <c r="M41" s="55">
+      <c r="M41" s="54">
         <f>M40+50</f>
         <v>365</v>
       </c>
-      <c r="N41" s="56"/>
+      <c r="N41" s="55"/>
       <c r="O41" s="16">
         <f>O40+50</f>
         <v>390</v>
@@ -4173,13 +5617,13 @@
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" s="42"/>
       <c r="C42" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D42" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>94</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>95</v>
       </c>
       <c r="F42" s="14" t="s">
         <v>47</v>
@@ -4200,11 +5644,11 @@
       <c r="K42" s="1">
         <v>70</v>
       </c>
-      <c r="M42" s="55">
+      <c r="M42" s="54">
         <f t="shared" ref="M42:M47" si="1">M41+50</f>
         <v>415</v>
       </c>
-      <c r="N42" s="56"/>
+      <c r="N42" s="55"/>
       <c r="O42" s="16">
         <f t="shared" ref="O42:O47" si="2">O41+50</f>
         <v>440</v>
@@ -4213,13 +5657,13 @@
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43" s="42"/>
       <c r="C43" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>97</v>
-      </c>
       <c r="E43" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F43" s="14" t="s">
         <v>47</v>
@@ -4240,11 +5684,11 @@
       <c r="K43" s="1">
         <v>110</v>
       </c>
-      <c r="M43" s="55">
+      <c r="M43" s="54">
         <f t="shared" si="1"/>
         <v>465</v>
       </c>
-      <c r="N43" s="56"/>
+      <c r="N43" s="55"/>
       <c r="O43" s="16">
         <f t="shared" si="2"/>
         <v>490</v>
@@ -4253,13 +5697,13 @@
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44" s="42"/>
       <c r="C44" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="13" t="s">
-        <v>97</v>
-      </c>
       <c r="E44" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F44" s="14" t="s">
         <v>47</v>
@@ -4280,11 +5724,11 @@
       <c r="K44" s="1">
         <v>110</v>
       </c>
-      <c r="M44" s="55">
+      <c r="M44" s="54">
         <f t="shared" si="1"/>
         <v>515</v>
       </c>
-      <c r="N44" s="56"/>
+      <c r="N44" s="55"/>
       <c r="O44" s="16">
         <f t="shared" si="2"/>
         <v>540</v>
@@ -4293,13 +5737,13 @@
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" s="42"/>
       <c r="C45" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="13" t="s">
-        <v>97</v>
-      </c>
       <c r="E45" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>47</v>
@@ -4320,11 +5764,11 @@
       <c r="K45" s="1">
         <v>110</v>
       </c>
-      <c r="M45" s="55">
+      <c r="M45" s="54">
         <f t="shared" si="1"/>
         <v>565</v>
       </c>
-      <c r="N45" s="56"/>
+      <c r="N45" s="55"/>
       <c r="O45" s="16">
         <f t="shared" si="2"/>
         <v>590</v>
@@ -4333,13 +5777,13 @@
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B46" s="42"/>
       <c r="C46" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F46" s="14" t="s">
         <v>47</v>
@@ -4360,11 +5804,11 @@
       <c r="K46" s="1">
         <v>150</v>
       </c>
-      <c r="M46" s="55">
+      <c r="M46" s="54">
         <f t="shared" si="1"/>
         <v>615</v>
       </c>
-      <c r="N46" s="56"/>
+      <c r="N46" s="55"/>
       <c r="O46" s="16">
         <f t="shared" si="2"/>
         <v>640</v>
@@ -4377,16 +5821,16 @@
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B47" s="42"/>
       <c r="C47" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D47" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E47" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E47" s="13" t="s">
-        <v>100</v>
-      </c>
       <c r="F47" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G47" s="14">
         <f t="shared" si="0"/>
@@ -4404,11 +5848,11 @@
       <c r="K47" s="1">
         <v>110</v>
       </c>
-      <c r="M47" s="55">
+      <c r="M47" s="54">
         <f t="shared" si="1"/>
         <v>665</v>
       </c>
-      <c r="N47" s="56"/>
+      <c r="N47" s="55"/>
       <c r="O47" s="16">
         <f t="shared" si="2"/>
         <v>690</v>
@@ -4417,16 +5861,16 @@
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B48" s="42"/>
       <c r="C48" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D48" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="E48" s="13" t="s">
-        <v>102</v>
-      </c>
       <c r="F48" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G48" s="14">
         <f t="shared" si="0"/>
@@ -4448,16 +5892,16 @@
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="42"/>
       <c r="C49" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D49" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="E49" s="13" t="s">
-        <v>104</v>
-      </c>
       <c r="F49" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G49" s="14">
         <f t="shared" si="0"/>
@@ -4477,18 +5921,18 @@
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="43"/>
+      <c r="B50" s="24"/>
       <c r="C50" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="E50" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E50" s="13" t="s">
+      <c r="F50" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>119</v>
       </c>
       <c r="G50" s="14">
         <f>IFERROR(VLOOKUP(I50,$E$2:$F$4,2,0)*8,0)+K50</f>
@@ -4505,6 +5949,37 @@
       </c>
       <c r="K50" s="1">
         <v>1480</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="62"/>
+      <c r="C51" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" s="14">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="H51" s="14">
+        <v>1</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J51" s="1">
+        <v>315</v>
+      </c>
+      <c r="K51" s="1">
+        <v>-15</v>
       </c>
     </row>
   </sheetData>
@@ -4530,10 +6005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6487C1D2-A674-4414-8299-37AC10F5B8E0}">
-  <dimension ref="P2:Q15"/>
+  <dimension ref="P2:Q19"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4544,90 +6019,114 @@
   <sheetData>
     <row r="2" spans="16:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P3" s="47" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q3" s="48"/>
+      <c r="P3" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q3" s="47"/>
     </row>
     <row r="4" spans="16:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="P4" s="49" t="str">
+      <c r="P4" s="48" t="str">
         <f>FRAMECALCULATOR!E1</f>
         <v>Desired Print Area</v>
       </c>
-      <c r="Q4" s="50" t="s">
-        <v>123</v>
+      <c r="Q4" s="49" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="16:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="P5" s="51" t="str">
+      <c r="P5" s="50" t="str">
         <f>FRAMECALCULATOR!E2</f>
         <v>X</v>
       </c>
-      <c r="Q5" s="52">
+      <c r="Q5" s="51">
         <f>FRAMECALCULATOR!F2</f>
         <v>315</v>
       </c>
     </row>
     <row r="6" spans="16:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="P6" s="53" t="str">
+      <c r="P6" s="52" t="str">
         <f>FRAMECALCULATOR!E3</f>
         <v>Y</v>
       </c>
-      <c r="Q6" s="54">
+      <c r="Q6" s="53">
         <f>FRAMECALCULATOR!F3</f>
         <v>315</v>
       </c>
     </row>
     <row r="9" spans="16:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="P9" s="45" t="s">
+      <c r="P9" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q9" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="Q9" s="45" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="10" spans="16:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="P10" s="44" t="s">
+      <c r="P10" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="Q10" s="46">
+      <c r="Q10" s="45">
         <f>Q5+25</f>
         <v>340</v>
       </c>
     </row>
     <row r="11" spans="16:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="P11" s="44" t="s">
+      <c r="P11" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="Q11" s="46">
+      <c r="Q11" s="45">
         <f>Q6+25</f>
         <v>340</v>
       </c>
     </row>
     <row r="13" spans="16:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="P13" s="45" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q13" s="45" t="s">
-        <v>123</v>
+      <c r="P13" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q13" s="44" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="16:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="P14" s="44" t="s">
+      <c r="P14" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="Q14" s="46">
+      <c r="Q14" s="45">
         <f>Q5+12</f>
         <v>327</v>
       </c>
     </row>
     <row r="15" spans="16:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="P15" s="44" t="s">
+      <c r="P15" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="Q15" s="46">
+      <c r="Q15" s="45">
         <f>Q6+-13</f>
         <v>302</v>
+      </c>
+    </row>
+    <row r="17" spans="16:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P17" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q17" s="44"/>
+    </row>
+    <row r="18" spans="16:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="P18" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="45">
+        <f>Q5-15</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="16:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="P19" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="45">
+        <f>Q6-15</f>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected HD X cross member dimension formula
</commit_message>
<xml_diff>
--- a/FrameCalculator.xlsx
+++ b/FrameCalculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="114_{04D01490-EE98-4F05-8C12-A1B4D3BC434B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5905CC0D-A039-4589-8FD9-2070CB178F57}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA53D410-7DD2-4547-9334-261E16E730C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{2DD4E541-7648-4A97-AB5A-A9C0E0660C31}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{2DD4E541-7648-4A97-AB5A-A9C0E0660C31}"/>
   </bookViews>
   <sheets>
     <sheet name="FRAMECALCULATOR" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -980,7 +980,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1125,11 +1125,368 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="58">
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFD1F810"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="medium">
@@ -1566,7 +1923,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>72572</xdr:colOff>
+      <xdr:colOff>72571</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>135477</xdr:rowOff>
     </xdr:to>
@@ -1677,7 +2034,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Olivier Royer-Tardif" refreshedDate="44120.501693981481" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="45" xr:uid="{5F61B17E-7DC0-4CFB-85E8-FF96C6C9113B}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Olivier Royer-Tardif" refreshedDate="44130.915966319444" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="45" xr:uid="{5F61B17E-7DC0-4CFB-85E8-FF96C6C9113B}">
   <cacheSource type="worksheet">
     <worksheetSource ref="C7:H52" sheet="FRAMECALCULATOR"/>
   </cacheSource>
@@ -1705,23 +2062,36 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Length mm" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="140" maxValue="4000" count="16">
-        <n v="420"/>
-        <n v="410"/>
-        <n v="880"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="140" maxValue="7600" count="29">
+        <n v="870"/>
+        <n v="860"/>
+        <n v="1330"/>
         <n v="140"/>
-        <n v="510"/>
-        <n v="260"/>
-        <n v="320"/>
-        <n v="431"/>
-        <n v="340"/>
-        <n v="400"/>
-        <n v="385"/>
-        <n v="450"/>
+        <n v="960"/>
+        <n v="710"/>
+        <n v="770"/>
+        <n v="881"/>
+        <n v="790"/>
+        <n v="850"/>
+        <n v="835"/>
+        <n v="900"/>
         <n v="150"/>
-        <n v="4000"/>
-        <n v="300"/>
-        <n v="315"/>
+        <n v="7600"/>
+        <n v="750"/>
+        <n v="385" u="1"/>
+        <n v="320" u="1"/>
+        <n v="420" u="1"/>
+        <n v="410" u="1"/>
+        <n v="510" u="1"/>
+        <n v="300" u="1"/>
+        <n v="400" u="1"/>
+        <n v="4000" u="1"/>
+        <n v="880" u="1"/>
+        <n v="315" u="1"/>
+        <n v="260" u="1"/>
+        <n v="431" u="1"/>
+        <n v="450" u="1"/>
+        <n v="340" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Qty" numFmtId="0">
@@ -2095,14 +2465,14 @@
     <s v="Track_XHD_2020Profile"/>
     <s v="X axis support for HD9 and HD12 only. Replaces Regular X Axis if HD version is selected."/>
     <x v="8"/>
-    <x v="15"/>
+    <x v="0"/>
     <n v="1"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B74C2BB5-BA82-419A-891C-9C4B9F44329D}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" showDataTips="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B74C2BB5-BA82-419A-891C-9C4B9F44329D}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" showDataTips="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="O7:Q34" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -2127,23 +2497,36 @@
       </extLst>
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="17">
+      <items count="30">
         <item x="12"/>
+        <item m="1" x="25"/>
+        <item m="1" x="16"/>
+        <item m="1" x="28"/>
+        <item m="1" x="15"/>
+        <item m="1" x="21"/>
+        <item m="1" x="18"/>
+        <item m="1" x="17"/>
+        <item m="1" x="27"/>
+        <item x="3"/>
+        <item m="1" x="26"/>
+        <item m="1" x="23"/>
+        <item m="1" x="19"/>
+        <item m="1" x="22"/>
+        <item m="1" x="20"/>
+        <item m="1" x="24"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
         <item x="5"/>
         <item x="6"/>
+        <item x="7"/>
         <item x="8"/>
+        <item x="9"/>
         <item x="10"/>
-        <item x="9"/>
-        <item x="1"/>
-        <item x="0"/>
         <item x="11"/>
-        <item x="3"/>
-        <item x="7"/>
-        <item x="2"/>
-        <item x="4"/>
         <item x="13"/>
         <item x="14"/>
-        <item x="15"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2156,39 +2539,39 @@
   <rowItems count="26">
     <i>
       <x/>
-      <x v="1"/>
+      <x v="20"/>
     </i>
     <i r="1">
-      <x v="2"/>
+      <x v="21"/>
     </i>
     <i r="1">
-      <x v="10"/>
+      <x v="22"/>
     </i>
     <i t="blank">
       <x/>
     </i>
     <i>
       <x v="1"/>
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
       <x v="9"/>
     </i>
     <i r="1">
-      <x v="11"/>
+      <x v="16"/>
     </i>
     <i r="1">
-      <x v="12"/>
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
     </i>
     <i t="blank">
       <x v="1"/>
     </i>
     <i>
       <x v="2"/>
-      <x v="5"/>
+      <x v="24"/>
     </i>
     <i t="blank">
       <x v="2"/>
@@ -2198,45 +2581,45 @@
       <x/>
     </i>
     <i r="1">
-      <x v="4"/>
+      <x v="25"/>
     </i>
     <i r="1">
-      <x v="8"/>
+      <x v="26"/>
     </i>
     <i t="blank">
       <x v="3"/>
     </i>
     <i>
       <x v="4"/>
-      <x v="8"/>
+      <x v="26"/>
     </i>
     <i t="blank">
       <x v="4"/>
     </i>
     <i>
       <x v="5"/>
-      <x v="13"/>
+      <x v="27"/>
     </i>
     <i t="blank">
       <x v="5"/>
     </i>
     <i>
       <x v="6"/>
-      <x v="3"/>
+      <x v="23"/>
     </i>
     <i t="blank">
       <x v="6"/>
     </i>
     <i>
       <x v="7"/>
-      <x v="14"/>
+      <x v="28"/>
     </i>
     <i t="blank">
       <x v="7"/>
     </i>
     <i>
       <x v="8"/>
-      <x v="15"/>
+      <x v="16"/>
     </i>
     <i t="blank">
       <x v="8"/>
@@ -2249,80 +2632,80 @@
     <dataField name="Sum of Qty" fld="5" baseField="4" baseItem="2"/>
   </dataFields>
   <formats count="29">
-    <format dxfId="28">
+    <format dxfId="57">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="56">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="55">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="54">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="53">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="52">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="51">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="50">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="49">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="48">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="47">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="46">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="45">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="44">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="43">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="13">
+    <format dxfId="42">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="41">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="40">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="39">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="38">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="37">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="36">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -2335,7 +2718,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -2349,7 +2732,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -2361,7 +2744,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -2375,7 +2758,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -2387,7 +2770,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="29">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -2705,8 +3088,8 @@
   </sheetPr>
   <dimension ref="B1:U52"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -2726,8 +3109,8 @@
     <col min="13" max="13" width="11.81640625" customWidth="1"/>
     <col min="14" max="14" width="1.26953125" customWidth="1"/>
     <col min="15" max="15" width="32.1796875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="13.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.1796875" customWidth="1"/>
     <col min="19" max="19" width="12.26953125" customWidth="1"/>
   </cols>
@@ -2747,7 +3130,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="5">
-        <v>315</v>
+        <v>765</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>108</v>
@@ -2760,7 +3143,7 @@
       </c>
       <c r="F3" s="6">
         <f>F2</f>
-        <v>315</v>
+        <v>765</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -2772,7 +3155,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="5">
-        <v>340</v>
+        <v>790</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>104</v>
@@ -2846,7 +3229,7 @@
       </c>
       <c r="G8" s="14">
         <f t="shared" ref="G8:G52" si="0">IFERROR(VLOOKUP(I8,$E$2:$F$4,2,0),0)+K8</f>
-        <v>420</v>
+        <v>870</v>
       </c>
       <c r="H8" s="14">
         <v>1</v>
@@ -2886,7 +3269,7 @@
       </c>
       <c r="G9" s="14">
         <f t="shared" si="0"/>
-        <v>420</v>
+        <v>870</v>
       </c>
       <c r="H9" s="14">
         <v>1</v>
@@ -2904,14 +3287,14 @@
       <c r="O9" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="37">
-        <v>260</v>
+      <c r="P9" s="15">
+        <v>710</v>
       </c>
       <c r="Q9" s="30">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:21" x14ac:dyDescent="0.35">
       <c r="C10" s="13" t="s">
         <v>16</v>
       </c>
@@ -2926,7 +3309,7 @@
       </c>
       <c r="G10" s="14">
         <f t="shared" si="0"/>
-        <v>410</v>
+        <v>860</v>
       </c>
       <c r="H10" s="14">
         <v>1</v>
@@ -2944,8 +3327,8 @@
       <c r="O10" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P10" s="38">
-        <v>320</v>
+      <c r="P10" s="15">
+        <v>770</v>
       </c>
       <c r="Q10" s="31">
         <v>2</v>
@@ -2966,7 +3349,7 @@
       </c>
       <c r="G11" s="14">
         <f t="shared" si="0"/>
-        <v>410</v>
+        <v>860</v>
       </c>
       <c r="H11" s="14">
         <v>1</v>
@@ -2985,7 +3368,7 @@
         <v>23</v>
       </c>
       <c r="P11" s="15">
-        <v>431</v>
+        <v>881</v>
       </c>
       <c r="Q11" s="31">
         <v>1</v>
@@ -3006,7 +3389,7 @@
       </c>
       <c r="G12" s="14">
         <f t="shared" si="0"/>
-        <v>420</v>
+        <v>870</v>
       </c>
       <c r="H12" s="14">
         <v>1</v>
@@ -3025,7 +3408,7 @@
       <c r="P12" s="15"/>
       <c r="Q12" s="31"/>
     </row>
-    <row r="13" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="13" t="s">
         <v>16</v>
       </c>
@@ -3040,7 +3423,7 @@
       </c>
       <c r="G13" s="14">
         <f t="shared" si="0"/>
-        <v>420</v>
+        <v>870</v>
       </c>
       <c r="H13" s="14">
         <v>1</v>
@@ -3058,11 +3441,11 @@
       <c r="O13" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="P13" s="37">
-        <v>410</v>
+      <c r="P13" s="40">
+        <v>140</v>
       </c>
       <c r="Q13" s="31">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="3:21" x14ac:dyDescent="0.35">
@@ -3080,7 +3463,7 @@
       </c>
       <c r="G14" s="14">
         <f t="shared" si="0"/>
-        <v>410</v>
+        <v>860</v>
       </c>
       <c r="H14" s="14">
         <v>1</v>
@@ -3098,14 +3481,14 @@
       <c r="O14" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="P14" s="39">
-        <v>420</v>
+      <c r="P14" s="15">
+        <v>870</v>
       </c>
       <c r="Q14" s="31">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="3:21" x14ac:dyDescent="0.35">
       <c r="C15" s="13" t="s">
         <v>16</v>
       </c>
@@ -3120,7 +3503,7 @@
       </c>
       <c r="G15" s="14">
         <f t="shared" si="0"/>
-        <v>410</v>
+        <v>860</v>
       </c>
       <c r="H15" s="14">
         <v>1</v>
@@ -3138,11 +3521,11 @@
       <c r="O15" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="P15" s="38">
-        <v>140</v>
+      <c r="P15" s="15">
+        <v>860</v>
       </c>
       <c r="Q15" s="31">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="3:21" x14ac:dyDescent="0.35">
@@ -3160,7 +3543,7 @@
       </c>
       <c r="G16" s="14">
         <f t="shared" si="0"/>
-        <v>420</v>
+        <v>870</v>
       </c>
       <c r="H16" s="14">
         <v>1</v>
@@ -3179,7 +3562,7 @@
         <v>19</v>
       </c>
       <c r="P16" s="15">
-        <v>880</v>
+        <v>1330</v>
       </c>
       <c r="Q16" s="31">
         <v>6</v>
@@ -3200,7 +3583,7 @@
       </c>
       <c r="G17" s="14">
         <f t="shared" si="0"/>
-        <v>410</v>
+        <v>860</v>
       </c>
       <c r="H17" s="14">
         <v>1</v>
@@ -3219,7 +3602,7 @@
         <v>19</v>
       </c>
       <c r="P17" s="15">
-        <v>510</v>
+        <v>960</v>
       </c>
       <c r="Q17" s="31">
         <v>3</v>
@@ -3240,7 +3623,7 @@
       </c>
       <c r="G18" s="14">
         <f t="shared" si="0"/>
-        <v>410</v>
+        <v>860</v>
       </c>
       <c r="H18" s="14">
         <v>1</v>
@@ -3275,7 +3658,7 @@
       </c>
       <c r="G19" s="14">
         <f t="shared" si="0"/>
-        <v>880</v>
+        <v>1330</v>
       </c>
       <c r="H19" s="14">
         <v>1</v>
@@ -3293,8 +3676,8 @@
       <c r="O19" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="P19" s="40">
-        <v>400</v>
+      <c r="P19" s="15">
+        <v>850</v>
       </c>
       <c r="Q19" s="31">
         <v>2</v>
@@ -3316,7 +3699,7 @@
       </c>
       <c r="G20" s="14">
         <f t="shared" si="0"/>
-        <v>880</v>
+        <v>1330</v>
       </c>
       <c r="H20" s="14">
         <v>1</v>
@@ -3335,7 +3718,7 @@
       <c r="P20" s="15"/>
       <c r="Q20" s="31"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="24"/>
       <c r="C21" s="13" t="s">
         <v>16</v>
@@ -3351,7 +3734,7 @@
       </c>
       <c r="G21" s="14">
         <f t="shared" si="0"/>
-        <v>880</v>
+        <v>1330</v>
       </c>
       <c r="H21" s="14">
         <v>1</v>
@@ -3369,7 +3752,7 @@
       <c r="O21" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="P21" s="37">
+      <c r="P21" s="40">
         <v>150</v>
       </c>
       <c r="Q21" s="31">
@@ -3392,7 +3775,7 @@
       </c>
       <c r="G22" s="14">
         <f t="shared" si="0"/>
-        <v>880</v>
+        <v>1330</v>
       </c>
       <c r="H22" s="14">
         <v>1</v>
@@ -3410,8 +3793,8 @@
       <c r="O22" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="P22" s="39">
-        <v>385</v>
+      <c r="P22" s="15">
+        <v>835</v>
       </c>
       <c r="Q22" s="31">
         <v>1</v>
@@ -3433,7 +3816,7 @@
       </c>
       <c r="G23" s="14">
         <f t="shared" si="0"/>
-        <v>410</v>
+        <v>860</v>
       </c>
       <c r="H23" s="14">
         <v>1</v>
@@ -3451,8 +3834,8 @@
       <c r="O23" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="P23" s="38">
-        <v>450</v>
+      <c r="P23" s="15">
+        <v>900</v>
       </c>
       <c r="Q23" s="31">
         <v>3</v>
@@ -3527,8 +3910,8 @@
       <c r="O25" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="P25" s="40">
-        <v>450</v>
+      <c r="P25" s="15">
+        <v>900</v>
       </c>
       <c r="Q25" s="31">
         <v>3</v>
@@ -3604,7 +3987,7 @@
         <v>117</v>
       </c>
       <c r="P27" s="15">
-        <v>4000</v>
+        <v>7600</v>
       </c>
       <c r="Q27" s="31">
         <v>1</v>
@@ -3626,7 +4009,7 @@
       </c>
       <c r="G28" s="14">
         <f t="shared" si="0"/>
-        <v>410</v>
+        <v>860</v>
       </c>
       <c r="H28" s="14">
         <v>1</v>
@@ -3660,7 +4043,7 @@
       </c>
       <c r="G29" s="14">
         <f t="shared" si="0"/>
-        <v>880</v>
+        <v>1330</v>
       </c>
       <c r="H29" s="14">
         <v>1</v>
@@ -3680,7 +4063,7 @@
         <v>125</v>
       </c>
       <c r="P29" s="15">
-        <v>340</v>
+        <v>790</v>
       </c>
       <c r="Q29" s="31">
         <v>1</v>
@@ -3702,7 +4085,7 @@
       </c>
       <c r="G30" s="14">
         <f t="shared" si="0"/>
-        <v>880</v>
+        <v>1330</v>
       </c>
       <c r="H30" s="14">
         <v>1</v>
@@ -3736,7 +4119,7 @@
       </c>
       <c r="G31" s="14">
         <f t="shared" si="0"/>
-        <v>510</v>
+        <v>960</v>
       </c>
       <c r="H31" s="14">
         <v>1</v>
@@ -3755,7 +4138,7 @@
         <v>124</v>
       </c>
       <c r="P31" s="15">
-        <v>300</v>
+        <v>750</v>
       </c>
       <c r="Q31" s="31">
         <v>1</v>
@@ -3777,7 +4160,7 @@
       </c>
       <c r="G32" s="14">
         <f t="shared" si="0"/>
-        <v>510</v>
+        <v>960</v>
       </c>
       <c r="H32" s="14">
         <v>1</v>
@@ -3811,7 +4194,7 @@
       </c>
       <c r="G33" s="14">
         <f t="shared" si="0"/>
-        <v>510</v>
+        <v>960</v>
       </c>
       <c r="H33" s="14">
         <v>1</v>
@@ -3830,7 +4213,7 @@
         <v>131</v>
       </c>
       <c r="P33" s="15">
-        <v>315</v>
+        <v>870</v>
       </c>
       <c r="Q33" s="31">
         <v>1</v>
@@ -3851,7 +4234,7 @@
       </c>
       <c r="G34" s="14">
         <f t="shared" si="0"/>
-        <v>260</v>
+        <v>710</v>
       </c>
       <c r="H34" s="14">
         <v>1</v>
@@ -3884,7 +4267,7 @@
       </c>
       <c r="G35" s="14">
         <f t="shared" si="0"/>
-        <v>260</v>
+        <v>710</v>
       </c>
       <c r="H35" s="14">
         <v>1</v>
@@ -3924,7 +4307,7 @@
       </c>
       <c r="G36" s="14">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>770</v>
       </c>
       <c r="H36" s="14">
         <v>1</v>
@@ -3964,7 +4347,7 @@
       </c>
       <c r="G37" s="14">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>770</v>
       </c>
       <c r="H37" s="14">
         <v>1</v>
@@ -4003,7 +4386,7 @@
       </c>
       <c r="G38" s="14">
         <f t="shared" si="0"/>
-        <v>431</v>
+        <v>881</v>
       </c>
       <c r="H38" s="14">
         <v>1</v>
@@ -4041,7 +4424,7 @@
       </c>
       <c r="G39" s="14">
         <f t="shared" si="0"/>
-        <v>340</v>
+        <v>790</v>
       </c>
       <c r="H39" s="14">
         <v>1</v>
@@ -4079,7 +4462,7 @@
       </c>
       <c r="G40" s="14">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>850</v>
       </c>
       <c r="H40" s="14">
         <v>1</v>
@@ -4117,7 +4500,7 @@
       </c>
       <c r="G41" s="14">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>850</v>
       </c>
       <c r="H41" s="14">
         <v>1</v>
@@ -4157,7 +4540,7 @@
       </c>
       <c r="G42" s="14">
         <f t="shared" si="0"/>
-        <v>385</v>
+        <v>835</v>
       </c>
       <c r="H42" s="14">
         <v>1</v>
@@ -4197,7 +4580,7 @@
       </c>
       <c r="G43" s="14">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="H43" s="14">
         <v>1</v>
@@ -4237,7 +4620,7 @@
       </c>
       <c r="G44" s="14">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="H44" s="14">
         <v>1</v>
@@ -4277,7 +4660,7 @@
       </c>
       <c r="G45" s="14">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="H45" s="14">
         <v>1</v>
@@ -4361,7 +4744,7 @@
       </c>
       <c r="G47" s="14">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="H47" s="14">
         <v>1</v>
@@ -4401,7 +4784,7 @@
       </c>
       <c r="G48" s="14">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="H48" s="14">
         <v>1</v>
@@ -4432,7 +4815,7 @@
       </c>
       <c r="G49" s="14">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="H49" s="14">
         <v>1</v>
@@ -4463,7 +4846,7 @@
       </c>
       <c r="G50" s="14">
         <f>IFERROR(VLOOKUP(I50,$E$2:$F$4,2,0)*8,0)+K50</f>
-        <v>4000</v>
+        <v>7600</v>
       </c>
       <c r="H50" s="14">
         <v>1</v>
@@ -4494,7 +4877,7 @@
       </c>
       <c r="G51" s="14">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>750</v>
       </c>
       <c r="H51" s="14">
         <v>1</v>
@@ -4525,7 +4908,7 @@
       </c>
       <c r="G52" s="14">
         <f t="shared" si="0"/>
-        <v>315</v>
+        <v>870</v>
       </c>
       <c r="H52" s="14">
         <v>1</v>
@@ -4536,8 +4919,8 @@
       <c r="J52" s="1">
         <v>315</v>
       </c>
-      <c r="K52" s="1">
-        <v>0</v>
+      <c r="K52" s="63">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -4568,7 +4951,7 @@
   </sheetPr>
   <dimension ref="P2:Q19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
@@ -4601,7 +4984,7 @@
       </c>
       <c r="Q5" s="51">
         <f>FRAMECALCULATOR!F2</f>
-        <v>315</v>
+        <v>765</v>
       </c>
     </row>
     <row r="6" spans="16:17" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -4611,7 +4994,7 @@
       </c>
       <c r="Q6" s="53">
         <f>FRAMECALCULATOR!F3</f>
-        <v>315</v>
+        <v>765</v>
       </c>
     </row>
     <row r="9" spans="16:17" ht="15.5" x14ac:dyDescent="0.35">
@@ -4628,7 +5011,7 @@
       </c>
       <c r="Q10" s="45">
         <f>Q5+25</f>
-        <v>340</v>
+        <v>790</v>
       </c>
     </row>
     <row r="11" spans="16:17" ht="21" x14ac:dyDescent="0.5">
@@ -4637,7 +5020,7 @@
       </c>
       <c r="Q11" s="45">
         <f>Q6+25</f>
-        <v>340</v>
+        <v>790</v>
       </c>
     </row>
     <row r="13" spans="16:17" ht="15.5" x14ac:dyDescent="0.35">
@@ -4654,7 +5037,7 @@
       </c>
       <c r="Q14" s="45">
         <f>Q5+12</f>
-        <v>327</v>
+        <v>777</v>
       </c>
     </row>
     <row r="15" spans="16:17" ht="21" x14ac:dyDescent="0.5">
@@ -4663,7 +5046,7 @@
       </c>
       <c r="Q15" s="45">
         <f>Q6+-13</f>
-        <v>302</v>
+        <v>752</v>
       </c>
     </row>
     <row r="17" spans="16:17" ht="15.5" x14ac:dyDescent="0.35">
@@ -4678,7 +5061,7 @@
       </c>
       <c r="Q18" s="45">
         <f>Q5-15</f>
-        <v>300</v>
+        <v>750</v>
       </c>
     </row>
     <row r="19" spans="16:17" ht="21" x14ac:dyDescent="0.5">
@@ -4687,7 +5070,7 @@
       </c>
       <c r="Q19" s="45">
         <f>Q6-15</f>
-        <v>300</v>
+        <v>750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>